<commit_message>
Admin interface is almost done.
</commit_message>
<xml_diff>
--- a/list_of_specialty.xlsx
+++ b/list_of_specialty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm-Workspace\doctor.appointment.app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E08907F-9B44-4165-B07B-6535AFEBEF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E787B871-9D86-4703-9554-0B06BFDBFAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{107BD413-E51D-420B-AD72-6D6D330CC6FD}"/>
+    <workbookView xWindow="0" yWindow="2720" windowWidth="14400" windowHeight="7360" xr2:uid="{107BD413-E51D-420B-AD72-6D6D330CC6FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B5CE45-AD44-4199-9604-098A7419B08B}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Changes in Admin And Doctors profile
</commit_message>
<xml_diff>
--- a/list_of_specialty.xlsx
+++ b/list_of_specialty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm-Workspace\doctor.appointment.app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E787B871-9D86-4703-9554-0B06BFDBFAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DA02F2-5EB9-48EB-A678-E5D64DEA5DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2720" windowWidth="14400" windowHeight="7360" xr2:uid="{107BD413-E51D-420B-AD72-6D6D330CC6FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{107BD413-E51D-420B-AD72-6D6D330CC6FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B5CE45-AD44-4199-9604-098A7419B08B}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>